<commit_message>
Traget Folder - Commensurate with Source
</commit_message>
<xml_diff>
--- a/data/Demo.xlsx
+++ b/data/Demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="797" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="797" firstSheet="13" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2219" uniqueCount="651">
   <si>
     <t>ID</t>
   </si>
@@ -1104,9 +1104,6 @@
   </si>
   <si>
     <t>WaitUntil</t>
-  </si>
-  <si>
-    <t>Value=Visit the Investors' Marketplace;CompareMode=Contains;Option=IgnoreCase;TotalWaitTime=30;WaitInterval=1000</t>
   </si>
   <si>
     <t>/html/body/header/div[1]/div/div[2]/ul/li[1]/a</t>
@@ -2548,17 +2545,17 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>649</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>650</v>
       </c>
       <c r="I2"/>
     </row>
@@ -4965,7 +4962,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>251</v>
@@ -5159,7 +5156,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>251</v>
@@ -6305,7 +6302,7 @@
         <v>39</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>340</v>
@@ -6338,13 +6335,13 @@
         <v>339</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>641</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>642</v>
       </c>
       <c r="I4" s="2" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
@@ -6452,7 +6449,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>40</v>
@@ -6477,7 +6474,7 @@
         <v>42</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I4" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6499,7 +6496,7 @@
         <v>43</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6518,10 +6515,10 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6533,17 +6530,17 @@
         <v>36</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6600,18 +6597,18 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK19"/>
+  <dimension ref="A1:AMK18"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="1"/>
-    <col min="2" max="2" width="12.7109375" style="1"/>
-    <col min="3" max="3" width="11.85546875" style="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" style="1"/>
     <col min="5" max="5" width="11.85546875" style="1"/>
     <col min="6" max="6" width="9" style="1"/>
@@ -6660,13 +6657,13 @@
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>340</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I19" si="0">"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <f t="shared" ref="I2:I18" si="0">"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
         <v>list.add(new String[] {"IBKRHome#",  "setVars",  "",  "",  "",  "",  "URL=http:www.interactivebrokers.com",  "Set up the site information"});</v>
       </c>
     </row>
@@ -6795,27 +6792,26 @@
         <v>343</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>352</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E8"/>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
+        <v>353</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "WaitUntil",  "PartialLinkText",  "Visit the Investors' Marketplace",  "",  "no",  "Value=Visit the Investors' Marketplace;CompareMode=Contains;Option=IgnoreCase;TotalWaitTime=30;WaitInterval=1000",  "Verify existence of a link to the Investors' Marketplace"});</v>
+        <v>list.add(new String[] {"IBKRHome#",  "verifyWebElement",  "Xpath",  "/html/body/header/div[1]/div/div[2]/ul/li[1]/a",  "GetText",  "",  "Value=English;Option=IgnoreCase",  "Verify the English language option exists"});</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -6823,26 +6819,22 @@
         <v>343</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>355</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="E9"/>
+      <c r="G9"/>
       <c r="H9" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="I9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "verifyWebElement",  "Xpath",  "/html/body/header/div[1]/div/div[2]/ul/li[1]/a",  "GetText",  "",  "Value=English;Option=IgnoreCase",  "Verify the English language option exists"});</v>
+        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "WHY IB",  "",  "",  "",  "Verify the WHY IB link exists"});</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -6856,16 +6848,16 @@
         <v>150</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E10"/>
       <c r="G10"/>
       <c r="H10" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="I10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "WHY IB",  "",  "",  "",  "Verify the WHY IB link exists"});</v>
+        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "PRICING",  "",  "",  "",  "Verify the PRICING link exists"});</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -6879,16 +6871,16 @@
         <v>150</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E11"/>
       <c r="G11"/>
       <c r="H11" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "PRICING",  "",  "",  "",  "Verify the PRICING link exists"});</v>
+        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "TRADING",  "",  "",  "",  "Verify the TRADING link exists"});</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -6902,16 +6894,16 @@
         <v>150</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E12"/>
       <c r="G12"/>
       <c r="H12" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "TRADING",  "",  "",  "",  "Verify the TRADING link exists"});</v>
+        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "EDUCATION",  "",  "",  "",  "Verify the EDUCATION link exists"});</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -6925,16 +6917,16 @@
         <v>150</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E13"/>
       <c r="G13"/>
       <c r="H13" s="3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "EDUCATION",  "",  "",  "",  "Verify the EDUCATION link exists"});</v>
+        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "ABOUT IB",  "",  "",  "",  "Verify the ABOUT IB link exists"});</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -6948,16 +6940,16 @@
         <v>150</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E14"/>
       <c r="G14"/>
       <c r="H14" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "ABOUT IB",  "",  "",  "",  "Verify the ABOUT IB link exists"});</v>
+        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "CONTACT US",  "",  "",  "",  "Verify the CONTACT US link exists"});</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -6965,22 +6957,26 @@
         <v>343</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="E15"/>
-      <c r="G15"/>
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" t="s">
+        <v>368</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>369</v>
+      </c>
       <c r="H15" s="3" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="I15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "CONTACT US",  "",  "",  "",  "Verify the CONTACT US link exists"});</v>
+        <v>list.add(new String[] {"IBKRHome#",  "verifyWebElement",  "Xpath",  "/html/body/header/div[1]/div/div[2]/ul/li[3]/a",  "GetText",  "",  "Value=LOG IN;CompareMode=Contains",  "Verify the Log In link exists"});</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -6988,26 +6984,21 @@
         <v>343</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" t="s">
-        <v>190</v>
-      </c>
-      <c r="D16" t="s">
-        <v>369</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>370</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="G16"/>
       <c r="H16" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "verifyWebElement",  "Xpath",  "/html/body/header/div[1]/div/div[2]/ul/li[3]/a",  "GetText",  "",  "Value=LOG IN;CompareMode=Contains",  "Verify the Log In link exists"});</v>
+        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "OPEN ACCOUNT",  "",  "",  "",  "Verify the OPEN ACCCOUNT link exists"});</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -7015,21 +7006,17 @@
         <v>343</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="G17"/>
+        <v>373</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>374</v>
+      </c>
       <c r="H17" s="3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "findElement",  "LinkText",  "OPEN ACCOUNT",  "",  "",  "",  "Verify the OPEN ACCCOUNT link exists"});</v>
+        <v>list.add(new String[] {"IBKRHome#",  "runJS",  "",  "",  "",  "",  "jsCode=document.getElementById("searchField").click()",  "Try to find the SEARCH by java script"});</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -7037,48 +7024,30 @@
         <v>343</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>374</v>
+        <v>322</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="I18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>list.add(new String[] {"IBKRHome#",  "runJS",  "",  "",  "",  "",  "jsCode=document.getElementById("searchField").click()",  "Try to find the SEARCH by java script"});</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="I19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>list.add(new String[] {"IBKRHome#",  "Wait",  "",  "",  "",  "",  "WaitTime=5",  "Wait a bit"});</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C15 C17:C19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16:C18 C2:C14">
       <formula1>Locator</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B18">
       <formula1>Action</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E18">
       <formula1>Query</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7105,32 +7074,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -7143,8 +7112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" activeCellId="1" sqref="F10:F11 D22"/>
+    <sheetView windowProtection="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7165,19 +7134,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E1" t="s">
         <v>385</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>386</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>387</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>388</v>
-      </c>
-      <c r="H1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -7193,36 +7162,36 @@
         <v>157</v>
       </c>
       <c r="E3" t="s">
+        <v>389</v>
+      </c>
+      <c r="F3" t="s">
         <v>390</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>391</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>392</v>
-      </c>
-      <c r="H3" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>393</v>
+      </c>
+      <c r="C4" t="s">
         <v>394</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>395</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>396</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>397</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>398</v>
-      </c>
-      <c r="H4" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -7230,56 +7199,56 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
+        <v>399</v>
+      </c>
+      <c r="E5" t="s">
         <v>400</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>396</v>
+      </c>
+      <c r="G5" t="s">
         <v>401</v>
       </c>
-      <c r="F5" t="s">
-        <v>397</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>402</v>
-      </c>
-      <c r="H5" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C6" t="s">
         <v>150</v>
       </c>
       <c r="E6" t="s">
+        <v>404</v>
+      </c>
+      <c r="F6" t="s">
         <v>405</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>407</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C7" t="s">
         <v>409</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>410</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>411</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="5" t="s">
         <v>412</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -7293,18 +7262,18 @@
         <v>58</v>
       </c>
       <c r="F8" t="s">
+        <v>413</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>414</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C9" t="s">
         <v>143</v>
@@ -7313,30 +7282,30 @@
         <v>140</v>
       </c>
       <c r="F9" t="s">
+        <v>416</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>418</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C10" t="s">
         <v>190</v>
       </c>
       <c r="E10" t="s">
+        <v>420</v>
+      </c>
+      <c r="F10" t="s">
         <v>421</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="5" t="s">
         <v>422</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -7344,20 +7313,20 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>424</v>
+      </c>
+      <c r="E12" t="s">
         <v>425</v>
-      </c>
-      <c r="E12" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -7372,22 +7341,22 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="20" spans="1:1">
@@ -7397,7 +7366,7 @@
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="22" spans="1:1">
@@ -7407,22 +7376,22 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="27" spans="1:1">
@@ -7470,27 +7439,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B1" t="s">
         <v>437</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>438</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>439</v>
-      </c>
-      <c r="D1" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B2" t="s">
         <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D2" t="s">
         <v>192</v>
@@ -7498,13 +7467,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B3" t="s">
         <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D3" t="s">
         <v>192</v>
@@ -7512,13 +7481,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D4" t="s">
         <v>192</v>
@@ -7526,7 +7495,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -7540,13 +7509,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D6" t="s">
         <v>192</v>
@@ -7554,13 +7523,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B7" t="s">
         <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D7" t="s">
         <v>192</v>
@@ -7568,7 +7537,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
@@ -7579,32 +7548,32 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
       </c>
       <c r="C9" t="s">
+        <v>452</v>
+      </c>
+      <c r="D9" t="s">
         <v>453</v>
-      </c>
-      <c r="D9" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B11" t="s">
         <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B12" t="s">
         <v>63</v>
@@ -7618,7 +7587,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B13" t="s">
         <v>63</v>
@@ -7632,12 +7601,12 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B15" t="s">
         <v>63</v>
@@ -7651,18 +7620,18 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B16" t="s">
         <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B17" t="s">
         <v>63</v>
@@ -7673,23 +7642,23 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B18" t="s">
         <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="C20" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="B21" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C21" t="s">
         <v>191</v>
@@ -7697,150 +7666,150 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>462</v>
+      </c>
+      <c r="B23" t="s">
         <v>463</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="3" t="s">
         <v>464</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>465</v>
+      </c>
+      <c r="B24" t="s">
         <v>466</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="9" t="s">
         <v>467</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>468</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>469</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" s="5"/>
       <c r="C27" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" s="5"/>
       <c r="C28" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B30" t="s">
         <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B31" t="s">
         <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B32" t="s">
         <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B33" t="s">
         <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="C34" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="C35" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="C36" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B37" t="s">
         <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B38" t="s">
         <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -7856,7 +7825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
@@ -7964,10 +7933,10 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>489</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>490</v>
       </c>
       <c r="I4" s="3" t="str">
         <f t="shared" si="0"/>
@@ -7992,7 +7961,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>266</v>
@@ -8379,7 +8348,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I20" s="3" t="str">
         <f t="shared" si="0"/>
@@ -8407,7 +8376,7 @@
         <v>320</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -8425,7 +8394,7 @@
         <v>325</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
@@ -8433,7 +8402,7 @@
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I22" s="3" t="str">
         <f t="shared" si="0"/>
@@ -8451,7 +8420,7 @@
         <v>325</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -8471,10 +8440,10 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I24" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A24 &amp; """" &amp; ",  " &amp; """" &amp; B24 &amp; """" &amp; ",  " &amp; """" &amp; C24 &amp; """" &amp; ",  " &amp; """" &amp; D24 &amp;  """" &amp;  ",  " &amp; """" &amp; E24 &amp; """" &amp; ",  " &amp; """" &amp; F24 &amp; """" &amp; ",  " &amp; """" &amp; G24 &amp; """" &amp; ",  " &amp; """" &amp; H24 &amp; """" &amp; "});"</f>
@@ -8496,7 +8465,7 @@
         <v>279</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I25" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A25 &amp; """" &amp; ",  " &amp; """" &amp; B25 &amp; """" &amp; ",  " &amp; """" &amp; C25 &amp; """" &amp; ",  " &amp; """" &amp; D25 &amp;  """" &amp;  ",  " &amp; """" &amp; E25 &amp; """" &amp; ",  " &amp; """" &amp; F25 &amp; """" &amp; ",  " &amp; """" &amp; G25 &amp; """" &amp; ",  " &amp; """" &amp; H25 &amp; """" &amp; "});"</f>
@@ -8518,7 +8487,7 @@
         <v>336</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I26" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A26 &amp; """" &amp; ",  " &amp; """" &amp; B26 &amp; """" &amp; ",  " &amp; """" &amp; C26 &amp; """" &amp; ",  " &amp; """" &amp; D26 &amp;  """" &amp;  ",  " &amp; """" &amp; E26 &amp; """" &amp; ",  " &amp; """" &amp; F26 &amp; """" &amp; ",  " &amp; """" &amp; G26 &amp; """" &amp; ",  " &amp; """" &amp; H26 &amp; """" &amp; "});"</f>
@@ -8554,10 +8523,10 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>499</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>500</v>
       </c>
       <c r="I28" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A28 &amp; """" &amp; ",  " &amp; """" &amp; B28 &amp; """" &amp; ",  " &amp; """" &amp; C28 &amp; """" &amp; ",  " &amp; """" &amp; D28 &amp;  """" &amp;  ",  " &amp; """" &amp; E28 &amp; """" &amp; ",  " &amp; """" &amp; F28 &amp; """" &amp; ",  " &amp; """" &amp; G28 &amp; """" &amp; ",  " &amp; """" &amp; H28 &amp; """" &amp; "});"</f>
@@ -8576,10 +8545,10 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>501</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>502</v>
       </c>
       <c r="I29" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A29 &amp; """" &amp; ",  " &amp; """" &amp; B29 &amp; """" &amp; ",  " &amp; """" &amp; C29 &amp; """" &amp; ",  " &amp; """" &amp; D29 &amp;  """" &amp;  ",  " &amp; """" &amp; E29 &amp; """" &amp; ",  " &amp; """" &amp; F29 &amp; """" &amp; ",  " &amp; """" &amp; G29 &amp; """" &amp; ",  " &amp; """" &amp; H29 &amp; """" &amp; "});"</f>
@@ -8598,10 +8567,10 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>503</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>504</v>
       </c>
       <c r="I30" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A30 &amp; """" &amp; ",  " &amp; """" &amp; B30 &amp; """" &amp; ",  " &amp; """" &amp; C30 &amp; """" &amp; ",  " &amp; """" &amp; D30 &amp;  """" &amp;  ",  " &amp; """" &amp; E30 &amp; """" &amp; ",  " &amp; """" &amp; F30 &amp; """" &amp; ",  " &amp; """" &amp; G30 &amp; """" &amp; ",  " &amp; """" &amp; H30 &amp; """" &amp; "});"</f>
@@ -8623,7 +8592,7 @@
         <v>279</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I31" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A31 &amp; """" &amp; ",  " &amp; """" &amp; B31 &amp; """" &amp; ",  " &amp; """" &amp; C31 &amp; """" &amp; ",  " &amp; """" &amp; D31 &amp;  """" &amp;  ",  " &amp; """" &amp; E31 &amp; """" &amp; ",  " &amp; """" &amp; F31 &amp; """" &amp; ",  " &amp; """" &amp; G31 &amp; """" &amp; ",  " &amp; """" &amp; H31 &amp; """" &amp; "});"</f>
@@ -8642,10 +8611,10 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="H32" s="3" t="s">
         <v>506</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>507</v>
       </c>
       <c r="I32" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A32 &amp; """" &amp; ",  " &amp; """" &amp; B32 &amp; """" &amp; ",  " &amp; """" &amp; C32 &amp; """" &amp; ",  " &amp; """" &amp; D32 &amp;  """" &amp;  ",  " &amp; """" &amp; E32 &amp; """" &amp; ",  " &amp; """" &amp; F32 &amp; """" &amp; ",  " &amp; """" &amp; G32 &amp; """" &amp; ",  " &amp; """" &amp; H32 &amp; """" &amp; "});"</f>
@@ -8680,13 +8649,13 @@
         <v>53</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I34" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A34 &amp; """" &amp; ",  " &amp; """" &amp; B34 &amp; """" &amp; ",  " &amp; """" &amp; C34 &amp; """" &amp; ",  " &amp; """" &amp; D34 &amp;  """" &amp;  ",  " &amp; """" &amp; E34 &amp; """" &amp; ",  " &amp; """" &amp; F34 &amp; """" &amp; ",  " &amp; """" &amp; G34 &amp; """" &amp; ",  " &amp; """" &amp; H34 &amp; """" &amp; "});"</f>
@@ -8705,7 +8674,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3" t="str">
@@ -8844,7 +8813,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>37</v>
@@ -8864,7 +8833,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>39</v>
@@ -8874,10 +8843,10 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I3" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
@@ -8886,7 +8855,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
@@ -8896,10 +8865,10 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>512</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>513</v>
       </c>
       <c r="I4" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
@@ -8908,7 +8877,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>41</v>
@@ -8920,7 +8889,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>255</v>
@@ -8997,7 +8966,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>45</v>
@@ -9007,7 +8976,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>47</v>
@@ -9019,7 +8988,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>48</v>
@@ -9031,7 +9000,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>51</v>
@@ -9043,7 +9012,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>56</v>
@@ -9052,17 +9021,17 @@
         <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>192</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>519</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>520</v>
       </c>
       <c r="I4" s="3" t="str">
         <f t="shared" si="0"/>
@@ -9071,7 +9040,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>56</v>
@@ -9080,14 +9049,14 @@
         <v>53</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>192</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>266</v>
@@ -9099,7 +9068,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>52</v>
@@ -9108,13 +9077,13 @@
         <v>150</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -9123,7 +9092,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>52</v>
@@ -9132,7 +9101,7 @@
         <v>150</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -9147,7 +9116,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>52</v>
@@ -9156,7 +9125,7 @@
         <v>150</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -9171,7 +9140,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>56</v>
@@ -9180,19 +9149,19 @@
         <v>53</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>528</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>529</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>530</v>
       </c>
       <c r="I9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -9201,7 +9170,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>56</v>
@@ -9210,19 +9179,19 @@
         <v>53</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>528</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>531</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>532</v>
       </c>
       <c r="I10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -9231,7 +9200,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>56</v>
@@ -9240,19 +9209,19 @@
         <v>53</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>528</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>533</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>534</v>
       </c>
       <c r="I11" s="3" t="str">
         <f t="shared" si="0"/>
@@ -9261,7 +9230,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>56</v>
@@ -9270,19 +9239,19 @@
         <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>528</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>535</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>536</v>
       </c>
       <c r="I12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -9291,7 +9260,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>56</v>
@@ -9300,19 +9269,19 @@
         <v>53</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>528</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>537</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>538</v>
       </c>
       <c r="I13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -9321,7 +9290,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>56</v>
@@ -9330,19 +9299,19 @@
         <v>53</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>528</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>539</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>540</v>
       </c>
       <c r="I14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -9351,7 +9320,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>56</v>
@@ -9360,19 +9329,19 @@
         <v>53</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>528</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>541</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>542</v>
       </c>
       <c r="I15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -9381,7 +9350,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>61</v>
@@ -9390,23 +9359,23 @@
         <v>53</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>528</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>56</v>
@@ -9415,17 +9384,17 @@
         <v>53</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>192</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>545</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>546</v>
       </c>
       <c r="I17" s="3" t="str">
         <f t="shared" ref="I17:I37" si="1">"list.add(new String[] {" &amp; """" &amp; A17 &amp; """" &amp; ",  " &amp; """" &amp; B17 &amp; """" &amp; ",  " &amp; """" &amp; C17 &amp; """" &amp; ",  " &amp; """" &amp; D17 &amp;  """" &amp;  ",  " &amp; """" &amp; E17 &amp; """" &amp; ",  " &amp; """" &amp; F17 &amp; """" &amp; ",  " &amp; """" &amp; G17 &amp; """" &amp; ",  " &amp; """" &amp; H17 &amp; """" &amp; "});"</f>
@@ -9434,7 +9403,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>52</v>
@@ -9443,7 +9412,7 @@
         <v>53</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
@@ -9462,7 +9431,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>52</v>
@@ -9471,7 +9440,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
@@ -9490,7 +9459,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>52</v>
@@ -9499,7 +9468,7 @@
         <v>53</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
@@ -9518,7 +9487,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>52</v>
@@ -9527,7 +9496,7 @@
         <v>53</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
@@ -9546,7 +9515,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>52</v>
@@ -9555,7 +9524,7 @@
         <v>53</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
@@ -9574,7 +9543,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>52</v>
@@ -9583,7 +9552,7 @@
         <v>53</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
@@ -9602,7 +9571,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>52</v>
@@ -9611,7 +9580,7 @@
         <v>53</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
@@ -9630,7 +9599,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>52</v>
@@ -9639,7 +9608,7 @@
         <v>53</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
@@ -9658,7 +9627,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>52</v>
@@ -9667,7 +9636,7 @@
         <v>53</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
@@ -9684,7 +9653,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>52</v>
@@ -9693,7 +9662,7 @@
         <v>53</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
@@ -9712,7 +9681,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>52</v>
@@ -9721,7 +9690,7 @@
         <v>53</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
@@ -9740,7 +9709,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>52</v>
@@ -9749,7 +9718,7 @@
         <v>53</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
@@ -9768,7 +9737,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>197</v>
@@ -9794,7 +9763,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>290</v>
@@ -9818,7 +9787,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>290</v>
@@ -9842,7 +9811,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>322</v>
@@ -9866,7 +9835,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>290</v>
@@ -9894,7 +9863,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>197</v>
@@ -9920,7 +9889,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>322</v>
@@ -9944,7 +9913,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>337</v>
@@ -10099,7 +10068,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -11152,10 +11121,10 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I2" s="3"/>
     </row>
@@ -11171,10 +11140,10 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I3" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
@@ -11193,10 +11162,10 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I4" s="3"/>
     </row>
@@ -11212,10 +11181,10 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I5" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
@@ -11234,10 +11203,10 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I6" s="3"/>
     </row>
@@ -11253,10 +11222,10 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I7" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A7 &amp; """" &amp; ",  " &amp; """" &amp; B7 &amp; """" &amp; ",  " &amp; """" &amp; C7 &amp; """" &amp; ",  " &amp; """" &amp; D7 &amp;  """" &amp;  ",  " &amp; """" &amp; E7 &amp; """" &amp; ",  " &amp; """" &amp; F7 &amp; """" &amp; ",  " &amp; """" &amp; G7 &amp; """" &amp; ",  " &amp; """" &amp; H7 &amp; """" &amp; "});"</f>
@@ -11275,10 +11244,10 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="12" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I8" s="3"/>
     </row>
@@ -11294,10 +11263,10 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I9" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A9 &amp; """" &amp; ",  " &amp; """" &amp; B9 &amp; """" &amp; ",  " &amp; """" &amp; C9 &amp; """" &amp; ",  " &amp; """" &amp; D9 &amp;  """" &amp;  ",  " &amp; """" &amp; E9 &amp; """" &amp; ",  " &amp; """" &amp; F9 &amp; """" &amp; ",  " &amp; """" &amp; G9 &amp; """" &amp; ",  " &amp; """" &amp; H9 &amp; """" &amp; "});"</f>
@@ -11316,10 +11285,10 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -11335,10 +11304,10 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I11" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A11 &amp; """" &amp; ",  " &amp; """" &amp; B11 &amp; """" &amp; ",  " &amp; """" &amp; C11 &amp; """" &amp; ",  " &amp; """" &amp; D11 &amp;  """" &amp;  ",  " &amp; """" &amp; E11 &amp; """" &amp; ",  " &amp; """" &amp; F11 &amp; """" &amp; ",  " &amp; """" &amp; G11 &amp; """" &amp; ",  " &amp; """" &amp; H11 &amp; """" &amp; "});"</f>
@@ -11357,10 +11326,10 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I12" s="3"/>
     </row>
@@ -11376,10 +11345,10 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I13" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A13 &amp; """" &amp; ",  " &amp; """" &amp; B13 &amp; """" &amp; ",  " &amp; """" &amp; C13 &amp; """" &amp; ",  " &amp; """" &amp; D13 &amp;  """" &amp;  ",  " &amp; """" &amp; E13 &amp; """" &amp; ",  " &amp; """" &amp; F13 &amp; """" &amp; ",  " &amp; """" &amp; G13 &amp; """" &amp; ",  " &amp; """" &amp; H13 &amp; """" &amp; "});"</f>
@@ -11398,10 +11367,10 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I14" s="3"/>
     </row>
@@ -11417,10 +11386,10 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I15" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A15 &amp; """" &amp; ",  " &amp; """" &amp; B15 &amp; """" &amp; ",  " &amp; """" &amp; C15 &amp; """" &amp; ",  " &amp; """" &amp; D15 &amp;  """" &amp;  ",  " &amp; """" &amp; E15 &amp; """" &amp; ",  " &amp; """" &amp; F15 &amp; """" &amp; ",  " &amp; """" &amp; G15 &amp; """" &amp; ",  " &amp; """" &amp; H15 &amp; """" &amp; "});"</f>
@@ -11439,10 +11408,10 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I16" s="3"/>
     </row>
@@ -11458,10 +11427,10 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I17" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A17 &amp; """" &amp; ",  " &amp; """" &amp; B17 &amp; """" &amp; ",  " &amp; """" &amp; C17 &amp; """" &amp; ",  " &amp; """" &amp; D17 &amp;  """" &amp;  ",  " &amp; """" &amp; E17 &amp; """" &amp; ",  " &amp; """" &amp; F17 &amp; """" &amp; ",  " &amp; """" &amp; G17 &amp; """" &amp; ",  " &amp; """" &amp; H17 &amp; """" &amp; "});"</f>
@@ -11480,10 +11449,10 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I18" s="3"/>
     </row>
@@ -11499,10 +11468,10 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I19" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A19 &amp; """" &amp; ",  " &amp; """" &amp; B19 &amp; """" &amp; ",  " &amp; """" &amp; C19 &amp; """" &amp; ",  " &amp; """" &amp; D19 &amp;  """" &amp;  ",  " &amp; """" &amp; E19 &amp; """" &amp; ",  " &amp; """" &amp; F19 &amp; """" &amp; ",  " &amp; """" &amp; G19 &amp; """" &amp; ",  " &amp; """" &amp; H19 &amp; """" &amp; "});"</f>
@@ -11521,10 +11490,10 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I20" s="3"/>
     </row>
@@ -11540,10 +11509,10 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I21" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A21 &amp; """" &amp; ",  " &amp; """" &amp; B21 &amp; """" &amp; ",  " &amp; """" &amp; C21 &amp; """" &amp; ",  " &amp; """" &amp; D21 &amp;  """" &amp;  ",  " &amp; """" &amp; E21 &amp; """" &amp; ",  " &amp; """" &amp; F21 &amp; """" &amp; ",  " &amp; """" &amp; G21 &amp; """" &amp; ",  " &amp; """" &amp; H21 &amp; """" &amp; "});"</f>
@@ -11562,10 +11531,10 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I22" s="3"/>
     </row>
@@ -11581,10 +11550,10 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I23" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A23 &amp; """" &amp; ",  " &amp; """" &amp; B23 &amp; """" &amp; ",  " &amp; """" &amp; C23 &amp; """" &amp; ",  " &amp; """" &amp; D23 &amp;  """" &amp;  ",  " &amp; """" &amp; E23 &amp; """" &amp; ",  " &amp; """" &amp; F23 &amp; """" &amp; ",  " &amp; """" &amp; G23 &amp; """" &amp; ",  " &amp; """" &amp; H23 &amp; """" &amp; "});"</f>
@@ -11603,10 +11572,10 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I24" s="3"/>
     </row>
@@ -11622,10 +11591,10 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I25" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A25 &amp; """" &amp; ",  " &amp; """" &amp; B25 &amp; """" &amp; ",  " &amp; """" &amp; C25 &amp; """" &amp; ",  " &amp; """" &amp; D25 &amp;  """" &amp;  ",  " &amp; """" &amp; E25 &amp; """" &amp; ",  " &amp; """" &amp; F25 &amp; """" &amp; ",  " &amp; """" &amp; G25 &amp; """" &amp; ",  " &amp; """" &amp; H25 &amp; """" &amp; "});"</f>
@@ -11644,10 +11613,10 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -11663,10 +11632,10 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I27" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A27 &amp; """" &amp; ",  " &amp; """" &amp; B27 &amp; """" &amp; ",  " &amp; """" &amp; C27 &amp; """" &amp; ",  " &amp; """" &amp; D27 &amp;  """" &amp;  ",  " &amp; """" &amp; E27 &amp; """" &amp; ",  " &amp; """" &amp; F27 &amp; """" &amp; ",  " &amp; """" &amp; G27 &amp; """" &amp; ",  " &amp; """" &amp; H27 &amp; """" &amp; "});"</f>
@@ -11685,10 +11654,10 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -11704,10 +11673,10 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I29" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A29 &amp; """" &amp; ",  " &amp; """" &amp; B29 &amp; """" &amp; ",  " &amp; """" &amp; C29 &amp; """" &amp; ",  " &amp; """" &amp; D29 &amp;  """" &amp;  ",  " &amp; """" &amp; E29 &amp; """" &amp; ",  " &amp; """" &amp; F29 &amp; """" &amp; ",  " &amp; """" &amp; G29 &amp; """" &amp; ",  " &amp; """" &amp; H29 &amp; """" &amp; "});"</f>
@@ -11726,10 +11695,10 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -11745,10 +11714,10 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I31" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A31 &amp; """" &amp; ",  " &amp; """" &amp; B31 &amp; """" &amp; ",  " &amp; """" &amp; C31 &amp; """" &amp; ",  " &amp; """" &amp; D31 &amp;  """" &amp;  ",  " &amp; """" &amp; E31 &amp; """" &amp; ",  " &amp; """" &amp; F31 &amp; """" &amp; ",  " &amp; """" &amp; G31 &amp; """" &amp; ",  " &amp; """" &amp; H31 &amp; """" &amp; "});"</f>
@@ -11767,10 +11736,10 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I32" s="3"/>
     </row>
@@ -11786,10 +11755,10 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I33" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A33 &amp; """" &amp; ",  " &amp; """" &amp; B33 &amp; """" &amp; ",  " &amp; """" &amp; C33 &amp; """" &amp; ",  " &amp; """" &amp; D33 &amp;  """" &amp;  ",  " &amp; """" &amp; E33 &amp; """" &amp; ",  " &amp; """" &amp; F33 &amp; """" &amp; ",  " &amp; """" &amp; G33 &amp; """" &amp; ",  " &amp; """" &amp; H33 &amp; """" &amp; "});"</f>
@@ -11808,10 +11777,10 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I34" s="3"/>
     </row>
@@ -11827,10 +11796,10 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I35" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A35 &amp; """" &amp; ",  " &amp; """" &amp; B35 &amp; """" &amp; ",  " &amp; """" &amp; C35 &amp; """" &amp; ",  " &amp; """" &amp; D35 &amp;  """" &amp;  ",  " &amp; """" &amp; E35 &amp; """" &amp; ",  " &amp; """" &amp; F35 &amp; """" &amp; ",  " &amp; """" &amp; G35 &amp; """" &amp; ",  " &amp; """" &amp; H35 &amp; """" &amp; "});"</f>
@@ -11918,7 +11887,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>61</v>
@@ -11927,15 +11896,15 @@
         <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I2" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
@@ -11944,7 +11913,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>61</v>
@@ -11953,15 +11922,15 @@
         <v>150</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I3" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
@@ -11970,7 +11939,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>139</v>
@@ -11979,15 +11948,15 @@
         <v>150</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I4" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
@@ -11996,7 +11965,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>212</v>
@@ -12008,10 +11977,10 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I5" s="3" t="str">
         <f t="shared" ref="I5:I9" si="0">"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
@@ -12020,7 +11989,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>322</v>
@@ -12033,7 +12002,7 @@
         <v>317</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12042,13 +12011,13 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>142</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>144</v>
@@ -12058,10 +12027,10 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I7" s="3" t="str">
         <f t="shared" ref="I7" si="1">"list.add(new String[] {" &amp; """" &amp; A7 &amp; """" &amp; ",  " &amp; """" &amp; B7 &amp; """" &amp; ",  " &amp; """" &amp; C7 &amp; """" &amp; ",  " &amp; """" &amp; D7 &amp;  """" &amp;  ",  " &amp; """" &amp; E7 &amp; """" &amp; ",  " &amp; """" &amp; F7 &amp; """" &amp; ",  " &amp; """" &amp; G7 &amp; """" &amp; ",  " &amp; """" &amp; H7 &amp; """" &amp; "});"</f>
@@ -12070,7 +12039,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>197</v>
@@ -12079,15 +12048,15 @@
         <v>150</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12096,7 +12065,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>212</v>
@@ -12108,7 +12077,7 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>141</v>
@@ -12199,7 +12168,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>61</v>
@@ -12208,15 +12177,15 @@
         <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I2" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
@@ -12225,7 +12194,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>61</v>
@@ -12234,15 +12203,15 @@
         <v>150</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I3" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
@@ -12251,7 +12220,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>139</v>
@@ -12260,15 +12229,15 @@
         <v>150</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I4" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
@@ -12277,7 +12246,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>212</v>
@@ -12289,10 +12258,10 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I5" s="3" t="str">
         <f t="shared" ref="I5:I7" si="0">"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
@@ -12301,7 +12270,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>322</v>
@@ -12314,7 +12283,7 @@
         <v>317</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12323,13 +12292,13 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>142</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>144</v>
@@ -12339,10 +12308,10 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12584,7 +12553,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>39</v>
@@ -12594,7 +12563,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="str">
@@ -12604,7 +12573,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>41</v>
@@ -12614,10 +12583,10 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I3" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
@@ -12626,24 +12595,24 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I4" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A4 &amp; """" &amp; ",  " &amp; """" &amp; B4 &amp; """" &amp; ",  " &amp; """" &amp; C4 &amp; """" &amp; ",  " &amp; """" &amp; D4 &amp;  """" &amp;  ",  " &amp; """" &amp; E4 &amp; """" &amp; ",  " &amp; """" &amp; F4 &amp; """" &amp; ",  " &amp; """" &amp; G4 &amp; """" &amp; ",  " &amp; """" &amp; H4 &amp; """" &amp; "});"</f>
@@ -12652,24 +12621,24 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I5" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A5 &amp; """" &amp; ",  " &amp; """" &amp; B5 &amp; """" &amp; ",  " &amp; """" &amp; C5 &amp; """" &amp; ",  " &amp; """" &amp; D5 &amp;  """" &amp;  ",  " &amp; """" &amp; E5 &amp; """" &amp; ",  " &amp; """" &amp; F5 &amp; """" &amp; ",  " &amp; """" &amp; G5 &amp; """" &amp; ",  " &amp; """" &amp; H5 &amp; """" &amp; "});"</f>
@@ -12678,24 +12647,24 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>592</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>593</v>
       </c>
       <c r="I6" s="3" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A6 &amp; """" &amp; ",  " &amp; """" &amp; B6 &amp; """" &amp; ",  " &amp; """" &amp; C6 &amp; """" &amp; ",  " &amp; """" &amp; D6 &amp;  """" &amp;  ",  " &amp; """" &amp; E6 &amp; """" &amp; ",  " &amp; """" &amp; F6 &amp; """" &amp; ",  " &amp; """" &amp; G6 &amp; """" &amp; ",  " &amp; """" &amp; H6 &amp; """" &amp; "});"</f>
@@ -12704,24 +12673,24 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>595</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>596</v>
       </c>
       <c r="I7" s="3" t="str">
         <f t="shared" ref="I7:I20" si="0">"list.add(new String[] {" &amp; """" &amp; A7 &amp; """" &amp; ",  " &amp; """" &amp; B7 &amp; """" &amp; ",  " &amp; """" &amp; C7 &amp; """" &amp; ",  " &amp; """" &amp; D7 &amp;  """" &amp;  ",  " &amp; """" &amp; E7 &amp; """" &amp; ",  " &amp; """" &amp; F7 &amp; """" &amp; ",  " &amp; """" &amp; G7 &amp; """" &amp; ",  " &amp; """" &amp; H7 &amp; """" &amp; "});"</f>
@@ -12730,24 +12699,24 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>598</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>599</v>
       </c>
       <c r="I8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12756,24 +12725,24 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>601</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>602</v>
       </c>
       <c r="I9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12782,24 +12751,24 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>604</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>605</v>
       </c>
       <c r="I10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12808,24 +12777,24 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>607</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>608</v>
       </c>
       <c r="I11" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12834,24 +12803,24 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>610</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>611</v>
       </c>
       <c r="I12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12860,24 +12829,24 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12886,24 +12855,24 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>615</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>616</v>
       </c>
       <c r="I14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12912,24 +12881,24 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12938,24 +12907,24 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12964,24 +12933,24 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I17" s="3" t="str">
         <f t="shared" si="0"/>
@@ -12990,24 +12959,24 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I18" s="3" t="str">
         <f t="shared" si="0"/>
@@ -13016,24 +12985,24 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -13042,24 +13011,24 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I20" s="3" t="str">
         <f t="shared" si="0"/>
@@ -13068,7 +13037,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>48</v>
@@ -13080,10 +13049,10 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I21" s="3" t="str">
         <f t="shared" ref="I21:I22" si="1">"list.add(new String[] {" &amp; """" &amp; A21 &amp; """" &amp; ",  " &amp; """" &amp; B21 &amp; """" &amp; ",  " &amp; """" &amp; C21 &amp; """" &amp; ",  " &amp; """" &amp; D21 &amp;  """" &amp;  ",  " &amp; """" &amp; E21 &amp; """" &amp; ",  " &amp; """" &amp; F21 &amp; """" &amp; ",  " &amp; """" &amp; G21 &amp; """" &amp; ",  " &amp; """" &amp; H21 &amp; """" &amp; "});"</f>
@@ -13092,7 +13061,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>322</v>
@@ -13105,7 +13074,7 @@
         <v>336</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I22" s="3" t="str">
         <f t="shared" si="1"/>
@@ -13723,9 +13692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="A24:XFD24"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13781,7 +13750,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>187</v>

</xml_diff>